<commit_message>
Reworked the HomePage entirely but looks pretty good the code logic is a bit sloppy so ill try to clean that up
</commit_message>
<xml_diff>
--- a/lib/menus/Bar 1.xlsx
+++ b/lib/menus/Bar 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chide/Desktop/barzzy_app2/lib/menus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB7ACF0-8B34-974A-B00D-C8EB8A44D008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76CEFF2-1231-6C46-BAD2-7B5640DA3E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{FA48C04F-F26E-274D-B83D-EDD113380032}"/>
   </bookViews>
@@ -179,9 +179,6 @@
     <t>This is a Casual Drink</t>
   </si>
   <si>
-    <t xml:space="preserve">The Burg Resto-Bar </t>
-  </si>
-  <si>
     <t>Casual</t>
   </si>
   <si>
@@ -222,6 +219,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Virginia, 24060, United States of America</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Burg </t>
   </si>
 </sst>
 </file>
@@ -307,7 +307,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -316,10 +320,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,32 +657,32 @@
   <dimension ref="A1:Q41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10" t="s">
+      <c r="A1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
@@ -691,29 +691,29 @@
       <c r="A2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
       <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
+      <c r="I2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
@@ -722,38 +722,38 @@
       <c r="A3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
       <c r="G3" s="2">
         <v>8.99</v>
       </c>
       <c r="H3" s="3">
         <v>0.45</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="K3" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="L3" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="M3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="N3" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
@@ -763,38 +763,38 @@
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="8"/>
+      <c r="D4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
       <c r="G4" s="2">
         <v>9.99</v>
       </c>
       <c r="H4" s="3">
         <v>0.45</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="K4" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="L4" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="M4" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="N4" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
@@ -804,38 +804,38 @@
       <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
       <c r="G5" s="2">
         <v>7.99</v>
       </c>
       <c r="H5" s="3">
         <v>0.45</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="K5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="L5" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="M5" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="N5" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
@@ -845,38 +845,38 @@
       <c r="A6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
       <c r="G6" s="2">
         <v>6.99</v>
       </c>
       <c r="H6" s="3">
         <v>0.45</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="K6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="L6" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="M6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="N6" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="N6" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
@@ -886,38 +886,38 @@
       <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
       <c r="G7" s="2">
         <v>8.99</v>
       </c>
       <c r="H7" s="3">
         <v>0.45</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="K7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="L7" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="M7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="N7" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
@@ -927,38 +927,38 @@
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7" t="s">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
       <c r="G8" s="2">
         <v>3.99</v>
       </c>
       <c r="H8" s="3">
         <v>0.45</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="K8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="L8" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="L8" s="11" t="s">
+      <c r="M8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="M8" s="11" t="s">
+      <c r="N8" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="N8" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
@@ -968,38 +968,38 @@
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7" t="s">
+      <c r="C9" s="8"/>
+      <c r="D9" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
       <c r="G9" s="2">
         <v>9.99</v>
       </c>
       <c r="H9" s="3">
         <v>0.45</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="K9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="L9" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="L9" s="11" t="s">
+      <c r="M9" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="M9" s="11" t="s">
+      <c r="N9" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="N9" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
@@ -1009,38 +1009,38 @@
       <c r="A10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7" t="s">
+      <c r="C10" s="8"/>
+      <c r="D10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="2">
         <v>10.99</v>
       </c>
       <c r="H10" s="3">
         <v>0.45</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="K10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="L10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="L10" s="11" t="s">
+      <c r="M10" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="M10" s="11" t="s">
+      <c r="N10" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="N10" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
@@ -1050,38 +1050,38 @@
       <c r="A11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7" t="s">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
       <c r="G11" s="2">
         <v>14.99</v>
       </c>
       <c r="H11" s="3">
         <v>0.45</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="K11" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="L11" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="L11" s="11" t="s">
+      <c r="M11" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="M11" s="11" t="s">
+      <c r="N11" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="N11" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
@@ -1091,38 +1091,38 @@
       <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7" t="s">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
       <c r="G12" s="2">
         <v>3.99</v>
       </c>
       <c r="H12" s="3">
         <v>0.45</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J12" s="11" t="s">
+      <c r="K12" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="K12" s="11" t="s">
+      <c r="L12" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="L12" s="11" t="s">
+      <c r="M12" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="M12" s="11" t="s">
+      <c r="N12" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="N12" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
@@ -1132,38 +1132,38 @@
       <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7" t="s">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="2">
         <v>6.99</v>
       </c>
       <c r="H13" s="3">
         <v>0.45</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J13" s="11" t="s">
+      <c r="K13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="K13" s="11" t="s">
+      <c r="L13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="L13" s="11" t="s">
+      <c r="M13" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="M13" s="11" t="s">
+      <c r="N13" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="N13" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
@@ -1173,38 +1173,38 @@
       <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7" t="s">
+      <c r="C14" s="8"/>
+      <c r="D14" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
       <c r="G14" s="2">
         <v>4.99</v>
       </c>
       <c r="H14" s="3">
         <v>0.45</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="I14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J14" s="11" t="s">
+      <c r="K14" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="K14" s="11" t="s">
+      <c r="L14" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="L14" s="11" t="s">
+      <c r="M14" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="M14" s="11" t="s">
+      <c r="N14" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="N14" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
@@ -1214,38 +1214,38 @@
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7" t="s">
+      <c r="C15" s="8"/>
+      <c r="D15" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="2">
         <v>4.99</v>
       </c>
       <c r="H15" s="3">
         <v>0.45</v>
       </c>
-      <c r="I15" s="11" t="s">
+      <c r="I15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J15" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J15" s="11" t="s">
+      <c r="K15" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="K15" s="11" t="s">
+      <c r="L15" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="L15" s="11" t="s">
+      <c r="M15" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="M15" s="11" t="s">
+      <c r="N15" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="N15" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
@@ -1255,38 +1255,38 @@
       <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7" t="s">
+      <c r="C16" s="8"/>
+      <c r="D16" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
       <c r="G16" s="2">
         <v>4.99</v>
       </c>
       <c r="H16" s="3">
         <v>0.45</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="I16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J16" s="11" t="s">
+      <c r="K16" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="K16" s="11" t="s">
+      <c r="L16" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="L16" s="11" t="s">
+      <c r="M16" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="M16" s="11" t="s">
+      <c r="N16" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="N16" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
@@ -1296,38 +1296,38 @@
       <c r="A17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="7" t="s">
+      <c r="C17" s="11"/>
+      <c r="D17" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
       <c r="G17" s="2">
         <v>4.99</v>
       </c>
       <c r="H17" s="3">
         <v>0</v>
       </c>
-      <c r="I17" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="L17" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="M17" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="N17" s="11" t="s">
-        <v>48</v>
+      <c r="I17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
@@ -1337,38 +1337,38 @@
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="7" t="s">
+      <c r="C18" s="11"/>
+      <c r="D18" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
       <c r="G18" s="2">
         <v>4.99</v>
       </c>
       <c r="H18" s="3">
         <v>0</v>
       </c>
-      <c r="I18" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="K18" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="L18" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="M18" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="N18" s="11" t="s">
-        <v>48</v>
+      <c r="I18" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
@@ -1378,38 +1378,38 @@
       <c r="A19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="7" t="s">
+      <c r="C19" s="11"/>
+      <c r="D19" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
       <c r="G19" s="2">
         <v>4.99</v>
       </c>
       <c r="H19" s="3">
         <v>0</v>
       </c>
-      <c r="I19" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="K19" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="L19" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="M19" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="N19" s="11" t="s">
-        <v>48</v>
+      <c r="I19" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
@@ -1419,38 +1419,38 @@
       <c r="A20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="7" t="s">
+      <c r="C20" s="11"/>
+      <c r="D20" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
       <c r="G20" s="2">
         <v>4.99</v>
       </c>
       <c r="H20" s="3">
         <v>0</v>
       </c>
-      <c r="I20" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="K20" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="L20" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="M20" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="N20" s="11" t="s">
-        <v>48</v>
+      <c r="I20" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
@@ -1458,40 +1458,40 @@
     </row>
     <row r="21" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="7" t="s">
+      <c r="C21" s="11"/>
+      <c r="D21" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
       <c r="G21" s="2">
         <v>4.99</v>
       </c>
       <c r="H21" s="3">
         <v>0.15</v>
       </c>
-      <c r="I21" s="11" t="s">
+      <c r="I21" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J21" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="J21" s="11" t="s">
+      <c r="K21" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="K21" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="L21" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="M21" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="N21" s="11" t="s">
-        <v>48</v>
+      <c r="L21" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
@@ -1499,40 +1499,40 @@
     </row>
     <row r="22" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="7" t="s">
+      <c r="C22" s="11"/>
+      <c r="D22" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
       <c r="G22" s="2">
         <v>4.99</v>
       </c>
       <c r="H22" s="3">
         <v>0.15</v>
       </c>
-      <c r="I22" s="11" t="s">
+      <c r="I22" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J22" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="J22" s="11" t="s">
+      <c r="K22" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="K22" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="L22" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="M22" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="N22" s="11" t="s">
-        <v>48</v>
+      <c r="L22" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
@@ -1540,40 +1540,40 @@
     </row>
     <row r="23" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="7" t="s">
+      <c r="C23" s="11"/>
+      <c r="D23" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
       <c r="G23" s="2">
         <v>4.99</v>
       </c>
       <c r="H23" s="3">
         <v>0.15</v>
       </c>
-      <c r="I23" s="11" t="s">
+      <c r="I23" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J23" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="J23" s="11" t="s">
+      <c r="K23" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="K23" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="L23" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="M23" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="N23" s="11" t="s">
-        <v>48</v>
+      <c r="L23" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
@@ -1581,40 +1581,40 @@
     </row>
     <row r="24" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="7" t="s">
+      <c r="C24" s="11"/>
+      <c r="D24" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
       <c r="G24" s="2">
         <v>4.99</v>
       </c>
       <c r="H24" s="3">
         <v>0.15</v>
       </c>
-      <c r="I24" s="11" t="s">
+      <c r="I24" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J24" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="J24" s="11" t="s">
+      <c r="K24" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="K24" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="L24" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="M24" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="N24" s="11" t="s">
-        <v>48</v>
+      <c r="L24" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="N24" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
@@ -1622,40 +1622,40 @@
     </row>
     <row r="25" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="7" t="s">
+      <c r="C25" s="11"/>
+      <c r="D25" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
       <c r="G25" s="2">
         <v>4.99</v>
       </c>
       <c r="H25" s="3">
         <v>0.15</v>
       </c>
-      <c r="I25" s="11" t="s">
+      <c r="I25" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J25" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="J25" s="11" t="s">
+      <c r="K25" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="K25" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="L25" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="M25" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="N25" s="11" t="s">
-        <v>48</v>
+      <c r="L25" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
@@ -1663,40 +1663,40 @@
     </row>
     <row r="26" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="7" t="s">
+      <c r="C26" s="11"/>
+      <c r="D26" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
       <c r="G26" s="2">
         <v>4.99</v>
       </c>
       <c r="H26" s="3">
         <v>0.15</v>
       </c>
-      <c r="I26" s="11" t="s">
+      <c r="I26" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J26" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="J26" s="11" t="s">
+      <c r="K26" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="K26" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="L26" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="M26" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="N26" s="11" t="s">
-        <v>48</v>
+      <c r="L26" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="M26" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="N26" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
@@ -1704,40 +1704,40 @@
     </row>
     <row r="27" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="7" t="s">
+      <c r="C27" s="11"/>
+      <c r="D27" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
       <c r="G27" s="2">
         <v>4.99</v>
       </c>
       <c r="H27" s="3">
         <v>0.15</v>
       </c>
-      <c r="I27" s="11" t="s">
+      <c r="I27" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J27" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="J27" s="11" t="s">
+      <c r="K27" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="K27" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="L27" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="M27" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="N27" s="11" t="s">
-        <v>48</v>
+      <c r="L27" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="M27" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="N27" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
@@ -1745,40 +1745,40 @@
     </row>
     <row r="28" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="7" t="s">
+      <c r="C28" s="11"/>
+      <c r="D28" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
       <c r="G28" s="2">
         <v>4.99</v>
       </c>
       <c r="H28" s="3">
         <v>0.15</v>
       </c>
-      <c r="I28" s="11" t="s">
+      <c r="I28" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J28" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="J28" s="11" t="s">
+      <c r="K28" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="K28" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="L28" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="M28" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="N28" s="11" t="s">
-        <v>48</v>
+      <c r="L28" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="M28" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="N28" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="O28" s="6"/>
       <c r="P28" s="6"/>
@@ -1786,40 +1786,40 @@
     </row>
     <row r="29" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="7" t="s">
+      <c r="C29" s="11"/>
+      <c r="D29" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
       <c r="G29" s="2">
         <v>4.99</v>
       </c>
       <c r="H29" s="3">
         <v>0.15</v>
       </c>
-      <c r="I29" s="11" t="s">
+      <c r="I29" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J29" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="J29" s="11" t="s">
+      <c r="K29" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="K29" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="L29" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="M29" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="N29" s="11" t="s">
-        <v>48</v>
+      <c r="L29" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="N29" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="O29" s="6"/>
       <c r="P29" s="6"/>
@@ -1827,40 +1827,40 @@
     </row>
     <row r="30" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="7" t="s">
+      <c r="C30" s="11"/>
+      <c r="D30" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
       <c r="G30" s="2">
         <v>4.99</v>
       </c>
       <c r="H30" s="3">
         <v>0.15</v>
       </c>
-      <c r="I30" s="11" t="s">
+      <c r="I30" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J30" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="J30" s="11" t="s">
+      <c r="K30" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="K30" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="L30" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="M30" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="N30" s="11" t="s">
-        <v>48</v>
+      <c r="L30" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="M30" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="O30" s="6"/>
       <c r="P30" s="6"/>
@@ -1868,40 +1868,40 @@
     </row>
     <row r="31" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="7" t="s">
+      <c r="C31" s="11"/>
+      <c r="D31" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
       <c r="G31" s="2">
         <v>4.99</v>
       </c>
       <c r="H31" s="3">
         <v>0.15</v>
       </c>
-      <c r="I31" s="11" t="s">
+      <c r="I31" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J31" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="J31" s="11" t="s">
+      <c r="K31" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="K31" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="L31" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="M31" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="N31" s="11" t="s">
-        <v>48</v>
+      <c r="L31" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="N31" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="O31" s="6"/>
       <c r="P31" s="6"/>
@@ -2021,38 +2021,22 @@
     </row>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="B11:C11"/>
@@ -2069,22 +2053,38 @@
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>